<commit_message>
added a few functions (see excel updates)
</commit_message>
<xml_diff>
--- a/PyPMT_progress.xlsx
+++ b/PyPMT_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Documents\GitHub\PyPMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C1BA6E-C378-4A5B-B304-E54EFA03E221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E58C16-FFEF-4839-B3AD-FAEFBC879451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1170" windowWidth="14400" windowHeight="7360" xr2:uid="{1B02746F-768C-4042-A572-64DD1F8AF2F8}"/>
+    <workbookView xWindow="80" yWindow="1170" windowWidth="14940" windowHeight="8110" xr2:uid="{1B02746F-768C-4042-A572-64DD1F8AF2F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Function</t>
   </si>
@@ -222,13 +222,22 @@
   </si>
   <si>
     <t>does not support rhumb line distances, as the MATLAB function does</t>
+  </si>
+  <si>
+    <t>Done??</t>
+  </si>
+  <si>
+    <t>in pypmt… had difficulty checking the test cases in matlab</t>
+  </si>
+  <si>
+    <t>same issue as pathdistps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +247,17 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF1B1642"/>
-      <name val="DM Sans"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,9 +280,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF2D08-B31E-4D2B-9726-DE919E241E43}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,6 +685,9 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -674,7 +696,7 @@
       <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -682,15 +704,30 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Forgot I did surfps a while ago
</commit_message>
<xml_diff>
--- a/PyPMT_progress.xlsx
+++ b/PyPMT_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Documents\GitHub\PyPMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F136FA87-B25C-4487-B708-FB534F972445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C92D9C7-6156-4213-9D4E-9DD341077C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="1170" windowWidth="14940" windowHeight="8110" xr2:uid="{1B02746F-768C-4042-A572-64DD1F8AF2F8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>Function</t>
   </si>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF2D08-B31E-4D2B-9726-DE919E241E43}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,6 +818,9 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
noted what functions are needed for certain tests
</commit_message>
<xml_diff>
--- a/PyPMT_progress.xlsx
+++ b/PyPMT_progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Documents\GitHub\PyPMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FEA9B5-4C10-40B3-9E9D-91E1CD2E5833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F155231-FAEC-4776-A2D5-7D52296EAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1170" windowWidth="14940" windowHeight="8110" xr2:uid="{1B02746F-768C-4042-A572-64DD1F8AF2F8}"/>
+    <workbookView xWindow="4410" yWindow="970" windowWidth="14940" windowHeight="8110" xr2:uid="{1B02746F-768C-4042-A572-64DD1F8AF2F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Function</t>
   </si>
@@ -240,6 +240,33 @@
   </si>
   <si>
     <t>tested on bedmachine plot just for fun (works)</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Needs scarlabel and scalebarps</t>
+  </si>
+  <si>
+    <t>needs mapzoomps to test</t>
+  </si>
+  <si>
+    <t>bedmap2 for testing</t>
+  </si>
+  <si>
+    <t>antmap, bedmap2, pcolorm for testing</t>
+  </si>
+  <si>
+    <t>pcolorps, graticuleps for testing</t>
+  </si>
+  <si>
+    <t>plotps for testing</t>
+  </si>
+  <si>
+    <t>needs patch, uistack for testing</t>
+  </si>
+  <si>
+    <t>needs antmap, pcolorm, bedmap2, quivermc, quiver for testing</t>
   </si>
 </sst>
 </file>
@@ -609,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF2D08-B31E-4D2B-9726-DE919E241E43}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,9 +645,10 @@
     <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -639,7 +667,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -647,7 +675,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -658,7 +686,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -668,8 +696,11 @@
       <c r="C5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -677,12 +708,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -690,7 +727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -698,7 +735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -709,7 +746,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -719,16 +756,22 @@
       <c r="C11" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -738,8 +781,11 @@
       <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -749,13 +795,16 @@
       <c r="C14" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -770,6 +819,9 @@
       <c r="B17" t="s">
         <v>51</v>
       </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -806,6 +858,12 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
adapted circleps to run with antbounds... trying to adapt scatterps but having issues
</commit_message>
<xml_diff>
--- a/PyPMT_progress.xlsx
+++ b/PyPMT_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Documents\GitHub\PyPMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D7F587-29A1-4F0D-AE84-346AE80F5F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9B25B8-DADE-4B28-811D-43F367403BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="0" windowWidth="14940" windowHeight="8110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
   <si>
     <t>Function</t>
   </si>
@@ -287,6 +287,21 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>Plot Compatible</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>fixing issues</t>
   </si>
 </sst>
 </file>
@@ -654,21 +669,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" customWidth="1"/>
+    <col min="4" max="4" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,26 +692,35 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -703,10 +728,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -714,13 +742,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -728,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -736,21 +767,27 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -758,114 +795,123 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -873,43 +919,43 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>45</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -917,18 +963,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>51</v>
       </c>
       <c r="B25" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -936,26 +982,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>57</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -963,7 +1012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -971,7 +1020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -979,18 +1028,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -998,36 +1047,45 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>65</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>67</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -1035,17 +1093,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -1053,17 +1114,20 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1071,23 +1135,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>76</v>
       </c>
       <c r="B46" t="s">
         <v>77</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -1095,31 +1159,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>80</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>81</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>82</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -1127,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -1135,7 +1208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -1143,12 +1216,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>86</v>
       </c>
       <c r="B54" t="s">
         <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added greenland_bounds... It works with other functions, but I still need to make the resolution better and add ice shelves
</commit_message>
<xml_diff>
--- a/PyPMT_progress.xlsx
+++ b/PyPMT_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Documents\GitHub\PyPMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E638DC-CDA3-4D55-BC7B-605A4CFAFA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9671D2E-218A-4EB5-B7FC-90C7B0AB1046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
   <si>
     <t>Function</t>
   </si>
@@ -184,12 +184,6 @@
     <t>pcolorps</t>
   </si>
   <si>
-    <t>Done (finally)</t>
-  </si>
-  <si>
-    <t>need to get in bedmap data to test</t>
-  </si>
-  <si>
     <t>surfps</t>
   </si>
   <si>
@@ -308,6 +302,9 @@
   </si>
   <si>
     <t>Problems</t>
+  </si>
+  <si>
+    <t>takes like 7-8 minutes though (for complete bedmachine data)</t>
   </si>
 </sst>
 </file>
@@ -677,15 +674,16 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -761,7 +759,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -973,15 +971,15 @@
         <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -989,32 +987,32 @@
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
         <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1022,7 +1020,7 @@
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -1030,26 +1028,26 @@
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
@@ -1057,45 +1055,45 @@
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -1103,41 +1101,41 @@
     </row>
     <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -1145,23 +1143,23 @@
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" t="s">
         <v>83</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -1169,7 +1167,7 @@
     </row>
     <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
@@ -1180,7 +1178,7 @@
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
@@ -1191,7 +1189,7 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
@@ -1202,7 +1200,7 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
@@ -1210,7 +1208,7 @@
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
@@ -1218,7 +1216,7 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -1226,7 +1224,7 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added graticuleps and plotps
</commit_message>
<xml_diff>
--- a/PyPMT_progress.xlsx
+++ b/PyPMT_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Documents\GitHub\PyPMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0EB875-0B09-4F43-99FC-B63DBED458C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3C8F37-9935-431C-A26A-9C2E551B70BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>Function</t>
   </si>
@@ -296,6 +296,18 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>need its_live and measures velocity data first</t>
+  </si>
+  <si>
+    <t>think it makes more sense to have mapzoom first</t>
+  </si>
+  <si>
+    <t>interactive (mouse clicks)</t>
+  </si>
+  <si>
+    <t>looks right??</t>
   </si>
 </sst>
 </file>
@@ -665,15 +677,15 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
   </cols>
@@ -933,7 +945,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
         <v>43</v>
@@ -1070,6 +1082,9 @@
       <c r="B33" t="s">
         <v>42</v>
       </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -1129,6 +1144,9 @@
       <c r="A40" t="s">
         <v>69</v>
       </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
@@ -1141,6 +1159,9 @@
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>